<commit_message>
add extract functions in py
changed the dir to tests file
</commit_message>
<xml_diff>
--- a/outputs/extracted_data/test.pdf.xlsx
+++ b/outputs/extracted_data/test.pdf.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +555,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Diesel consumption</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Diesel consumption</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Diesel consumption</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Company fleet mileage</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Company fleet mileage</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Company fleet mileage</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -723,12 +723,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Total electricity consumption</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>MWh</t>
+          <t>MWhs</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -751,12 +751,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Total electricity consumption</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MWh</t>
+          <t>MWhs</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -779,12 +779,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Total electricity consumption</t>
+          <t>Total energy consumption</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>MWh</t>
+          <t>MWhs</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -802,17 +802,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Greenhouse Gas Emissions</t>
+          <t>Energy Consumption</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Energy consumption intensity</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>tCO2e</t>
+          <t>MWhs</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>27497</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="15">
@@ -830,17 +830,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Greenhouse Gas Emissions</t>
+          <t>Energy Consumption</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Energy consumption intensity</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>tCO2e</t>
+          <t>MWhs</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -849,7 +849,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>65488</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="16">
@@ -858,17 +858,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Greenhouse Gas Emissions</t>
+          <t>Energy Consumption</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Energy consumption intensity</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>tCO2e</t>
+          <t>MWhs</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>68151</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="17">
@@ -891,7 +891,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Scope 1</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>147</v>
+        <v>27497</v>
       </c>
     </row>
     <row r="18">
@@ -919,7 +919,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Scope 1</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -933,7 +933,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>160</v>
+        <v>65488</v>
       </c>
     </row>
     <row r="19">
@@ -947,7 +947,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Scope 1</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -961,7 +961,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>237</v>
+        <v>68151</v>
       </c>
     </row>
     <row r="20">
@@ -975,7 +975,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Scope 2</t>
+          <t>Scope 1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -989,7 +989,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>68334</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Scope 2</t>
+          <t>Scope 1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>63811</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Scope 2</t>
+          <t>Scope 1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>67636</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Scope 3</t>
+          <t>Scope 2</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1073,7 +1073,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>3849</v>
+        <v>68334</v>
       </c>
     </row>
     <row r="24">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Scope 3</t>
+          <t>Scope 2</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1517</v>
+        <v>63811</v>
       </c>
     </row>
     <row r="25">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Scope 3</t>
+          <t>Scope 2</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1129,7 +1129,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>278</v>
+        <v>67636</v>
       </c>
     </row>
     <row r="26">
@@ -1138,17 +1138,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Water Consumption</t>
+          <t>Greenhouse Gas Emissions</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Total water consumption</t>
+          <t>Scope 3</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>m³</t>
+          <t>tCO2e</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>433969</v>
+        <v>3849</v>
       </c>
     </row>
     <row r="27">
@@ -1166,17 +1166,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Water Consumption</t>
+          <t>Greenhouse Gas Emissions</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Total water consumption</t>
+          <t>Scope 3</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>m³</t>
+          <t>tCO2e</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>400322</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="28">
@@ -1194,17 +1194,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Water Consumption</t>
+          <t>Greenhouse Gas Emissions</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Total water consumption</t>
+          <t>Scope 3</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>m³</t>
+          <t>tCO2e</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>407051</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29">
@@ -1222,17 +1222,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Water Consumption</t>
+          <t>Greenhouse Gas Emissions</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Water consumption intensity</t>
+          <t>Emission intensities of Scope 2</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>m³/ft2</t>
+          <t>tCO2e</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0.101</v>
+        <v>0.0123</v>
       </c>
     </row>
     <row r="30">
@@ -1250,17 +1250,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Water Consumption</t>
+          <t>Greenhouse Gas Emissions</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Water consumption intensity</t>
+          <t>Emission intensities of Scope 2</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>m³/ft2</t>
+          <t>tCO2e</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>0.097</v>
+        <v>0.0115</v>
       </c>
     </row>
     <row r="31">
@@ -1278,17 +1278,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Waste Generation</t>
+          <t>Water Consumption</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Total waste generated</t>
+          <t>Total water consumption</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1605</v>
+        <v>433969</v>
       </c>
     </row>
     <row r="32">
@@ -1306,17 +1306,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Waste Generation</t>
+          <t>Water Consumption</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Total waste generated</t>
+          <t>Total water consumption</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1325,7 +1325,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1229</v>
+        <v>400322</v>
       </c>
     </row>
     <row r="33">
@@ -1334,26 +1334,166 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>Water Consumption</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Total water consumption</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>m³</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>407051</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Water Consumption</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Water consumption intensity</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>m³</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>0.101</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Water Consumption</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Water consumption intensity</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>m³</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>0.097</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Water Consumption</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Water consumption intensity</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>m³</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>0.077</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>Waste Generation</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>Total waste generated</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>t</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>379</v>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Waste Generation</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Total waste generated</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>1229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>